<commit_message>
added data for 4 BJs, 4 machines
git-svn-id: file://localhost/tmp/svn2git/svn@2997 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/async-re/data/Refined_data.xlsx
+++ b/papers/async-re/data/Refined_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t>Synchronous</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -82,6 +82,82 @@
   </si>
   <si>
     <t>1B. 16 ex, 2 machines</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4BJS 4 MACHINES</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERIC, LOUIE, OLIVER, POSEIDON, OLIVER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>diff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>se</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>decent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>diff</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>se</t>
+  </si>
+  <si>
+    <t>SE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gap b/w 1st and last bjs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1BJ 8 Reps/32 exchanges</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1BJ 16 Reps/64 ex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1BJ 32 Reps/128 ex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4BJs, 4Machines - 16 replicas/64 exchanges</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -475,24 +551,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="532704760"/>
-        <c:axId val="610933784"/>
+        <c:axId val="464178680"/>
+        <c:axId val="478299880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="532704760"/>
+        <c:axId val="464178680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="610933784"/>
+        <c:crossAx val="478299880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="610933784"/>
+        <c:axId val="478299880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -500,7 +576,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="532704760"/>
+        <c:crossAx val="464178680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -837,11 +913,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="528194616"/>
-        <c:axId val="532888760"/>
+        <c:axId val="501251624"/>
+        <c:axId val="478372568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="528194616"/>
+        <c:axId val="501251624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -865,14 +941,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="532888760"/>
+        <c:crossAx val="478372568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="532888760"/>
+        <c:axId val="478372568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -880,7 +956,302 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="528194616"/>
+        <c:crossAx val="501251624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>LONI machines</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$97</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Asynchronous - Centralized</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(Sheet1!$C$97,Sheet1!$E$97,Sheet1!$G$97,Sheet1!$I$97)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>7.11</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.23</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>16.36</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>13.4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(Sheet1!$C$97,Sheet1!$E$97,Sheet1!$G$97,Sheet1!$I$97)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>7.11</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.23</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>16.36</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>13.4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Sheet1!$B$96,Sheet1!$D$96,Sheet1!$F$96,Sheet1!$H$96)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4BJs, 4Machines - 16 replicas/64 exchanges</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1BJ 8 Reps/32 exchanges</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1BJ 16 Reps/64 ex</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1BJ 32 Reps/128 ex</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Sheet1!$B$97,Sheet1!$D$97,Sheet1!$F$97,Sheet1!$H$97)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>685.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>630.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>701.83</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>804.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$98</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Asynchronous - Decentralized</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(Sheet1!$C$98,Sheet1!$E$98,Sheet1!$G$98,Sheet1!$I$98)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>1.66</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>6.14</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3.38</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4.24</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(Sheet1!$C$98,Sheet1!$E$98,Sheet1!$G$98,Sheet1!$I$98)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>1.66</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>6.14</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3.38</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4.24</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Sheet1!$B$96,Sheet1!$D$96,Sheet1!$F$96,Sheet1!$H$96)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4BJs, 4Machines - 16 replicas/64 exchanges</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1BJ 8 Reps/32 exchanges</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1BJ 16 Reps/64 ex</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1BJ 32 Reps/128 ex</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Sheet1!$B$98,Sheet1!$D$98,Sheet1!$F$98,Sheet1!$H$98)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>641.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>609.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>583.33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>641.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="524606536"/>
+        <c:axId val="524797800"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="524606536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="524797800"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="524797800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Mean runtime, seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="524606536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -956,6 +1327,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1727,10 +2128,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="M73" sqref="M73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1996,7 +2397,469 @@
         <v>6.14</v>
       </c>
     </row>
+    <row r="73" spans="1:9">
+      <c r="A73" t="s">
+        <v>16</v>
+      </c>
+      <c r="C73" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="B75">
+        <v>64</v>
+      </c>
+      <c r="C75">
+        <v>65</v>
+      </c>
+      <c r="D75">
+        <v>66</v>
+      </c>
+      <c r="E75">
+        <v>67</v>
+      </c>
+      <c r="F75">
+        <v>68</v>
+      </c>
+      <c r="G75">
+        <v>69</v>
+      </c>
+      <c r="H75">
+        <v>70</v>
+      </c>
+      <c r="I75">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" t="s">
+        <v>31</v>
+      </c>
+      <c r="B76">
+        <v>50</v>
+      </c>
+      <c r="C76">
+        <v>40</v>
+      </c>
+      <c r="E76">
+        <v>50</v>
+      </c>
+      <c r="F76">
+        <v>60</v>
+      </c>
+      <c r="G76">
+        <v>40</v>
+      </c>
+      <c r="H76">
+        <v>60</v>
+      </c>
+      <c r="I76">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" t="s">
+        <v>18</v>
+      </c>
+      <c r="B77">
+        <v>665</v>
+      </c>
+      <c r="C77">
+        <v>703</v>
+      </c>
+      <c r="E77">
+        <v>668</v>
+      </c>
+      <c r="F77">
+        <v>713</v>
+      </c>
+      <c r="G77">
+        <v>663</v>
+      </c>
+      <c r="H77">
+        <v>687</v>
+      </c>
+      <c r="I77">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78" t="s">
+        <v>19</v>
+      </c>
+      <c r="B78">
+        <v>685.42857142857144</v>
+      </c>
+      <c r="C78">
+        <v>685.42857142857144</v>
+      </c>
+      <c r="E78">
+        <v>685.42857142857144</v>
+      </c>
+      <c r="F78">
+        <v>685.42857142857144</v>
+      </c>
+      <c r="G78">
+        <v>685.42857142857144</v>
+      </c>
+      <c r="H78">
+        <v>685.42857142857144</v>
+      </c>
+      <c r="I78">
+        <v>685.42857142857144</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79" t="s">
+        <v>20</v>
+      </c>
+      <c r="B79">
+        <f>(B77-B78)*(B77-B78)</f>
+        <v>417.32653061224556</v>
+      </c>
+      <c r="C79">
+        <f t="shared" ref="C79" si="0">(C77-C78)*(C77-C78)</f>
+        <v>308.75510204081576</v>
+      </c>
+      <c r="E79">
+        <f>(E77-E78)*(E77-E78)</f>
+        <v>303.75510204081689</v>
+      </c>
+      <c r="F79">
+        <f>(F77-F78)*(F77-F78)</f>
+        <v>760.1836734693868</v>
+      </c>
+      <c r="G79">
+        <f>(G77-G78)*(G77-G78)</f>
+        <v>503.04081632653134</v>
+      </c>
+      <c r="H79">
+        <f>(H77-H78)*(H77-H78)</f>
+        <v>2.4693877551019896</v>
+      </c>
+      <c r="I79">
+        <f>(I77-I78)*(I77-I78)</f>
+        <v>184.18367346938732</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80" t="s">
+        <v>21</v>
+      </c>
+      <c r="B80">
+        <v>18.82139468687652</v>
+      </c>
+      <c r="C80">
+        <v>18.82139468687652</v>
+      </c>
+      <c r="E80">
+        <v>18.82139468687652</v>
+      </c>
+      <c r="F80">
+        <v>18.82139468687652</v>
+      </c>
+      <c r="G80">
+        <v>18.82139468687652</v>
+      </c>
+      <c r="H80">
+        <v>18.82139468687652</v>
+      </c>
+      <c r="I80">
+        <v>18.82139468687652</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81" t="s">
+        <v>22</v>
+      </c>
+      <c r="B81">
+        <f>B80/SQRT(7)</f>
+        <v>7.1138185241239524</v>
+      </c>
+      <c r="C81">
+        <f t="shared" ref="C81" si="1">C80/SQRT(7)</f>
+        <v>7.1138185241239524</v>
+      </c>
+      <c r="E81">
+        <f>E80/SQRT(7)</f>
+        <v>7.1138185241239524</v>
+      </c>
+      <c r="F81">
+        <f>F80/SQRT(7)</f>
+        <v>7.1138185241239524</v>
+      </c>
+      <c r="G81">
+        <f>G80/SQRT(7)</f>
+        <v>7.1138185241239524</v>
+      </c>
+      <c r="H81">
+        <f>H80/SQRT(7)</f>
+        <v>7.1138185241239524</v>
+      </c>
+      <c r="I81">
+        <f>I80/SQRT(7)</f>
+        <v>7.1138185241239524</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="B84">
+        <v>61</v>
+      </c>
+      <c r="C84">
+        <v>62</v>
+      </c>
+      <c r="D84">
+        <v>63</v>
+      </c>
+      <c r="E84">
+        <v>64</v>
+      </c>
+      <c r="F84">
+        <v>65</v>
+      </c>
+      <c r="G84">
+        <v>66</v>
+      </c>
+      <c r="H84">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85" t="s">
+        <v>23</v>
+      </c>
+      <c r="C85">
+        <v>64</v>
+      </c>
+      <c r="D85">
+        <v>40</v>
+      </c>
+      <c r="E85">
+        <v>45</v>
+      </c>
+      <c r="F85">
+        <v>45</v>
+      </c>
+      <c r="G85">
+        <v>20</v>
+      </c>
+      <c r="H85">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="A86" t="s">
+        <v>24</v>
+      </c>
+      <c r="C86">
+        <v>626</v>
+      </c>
+      <c r="D86">
+        <v>635</v>
+      </c>
+      <c r="E86">
+        <v>656</v>
+      </c>
+      <c r="F86">
+        <v>632</v>
+      </c>
+      <c r="G86">
+        <v>643</v>
+      </c>
+      <c r="H86">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
+      <c r="A87" t="s">
+        <v>25</v>
+      </c>
+      <c r="C87">
+        <v>641.16666666666663</v>
+      </c>
+      <c r="D87">
+        <v>641.16666666666663</v>
+      </c>
+      <c r="E87">
+        <v>641.16666666666663</v>
+      </c>
+      <c r="F87">
+        <v>641.16666666666663</v>
+      </c>
+      <c r="G87">
+        <v>641.16666666666663</v>
+      </c>
+      <c r="H87">
+        <v>641.16666666666663</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
+      <c r="A88" t="s">
+        <v>26</v>
+      </c>
+      <c r="C88">
+        <f>(C87-C86)*(C87-C86)</f>
+        <v>230.02777777777663</v>
+      </c>
+      <c r="D88">
+        <f t="shared" ref="D88" si="2">(D87-D86)*(D87-D86)</f>
+        <v>38.02777777777731</v>
+      </c>
+      <c r="E88">
+        <f>(E87-E86)*(E87-E86)</f>
+        <v>220.02777777777891</v>
+      </c>
+      <c r="F88">
+        <f>(F87-F86)*(F87-F86)</f>
+        <v>84.027777777777089</v>
+      </c>
+      <c r="G88">
+        <f>(G87-G86)*(G87-G86)</f>
+        <v>3.3611111111112502</v>
+      </c>
+      <c r="H88">
+        <f>(H87-H86)*(H87-H86)</f>
+        <v>191.36111111111217</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9">
+      <c r="A89" t="s">
+        <v>27</v>
+      </c>
+      <c r="C89">
+        <v>4.0767952444565694</v>
+      </c>
+      <c r="D89">
+        <v>4.0767952444565694</v>
+      </c>
+      <c r="E89">
+        <v>4.0767952444565694</v>
+      </c>
+      <c r="F89">
+        <v>4.0767952444565694</v>
+      </c>
+      <c r="G89">
+        <v>4.0767952444565694</v>
+      </c>
+      <c r="H89">
+        <v>4.0767952444565694</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
+      <c r="A90" t="s">
+        <v>28</v>
+      </c>
+      <c r="C90">
+        <f>C89/SQRT(6)</f>
+        <v>1.6643446891206011</v>
+      </c>
+      <c r="D90">
+        <f t="shared" ref="D90" si="3">D89/SQRT(6)</f>
+        <v>1.6643446891206011</v>
+      </c>
+      <c r="E90">
+        <f>E89/SQRT(6)</f>
+        <v>1.6643446891206011</v>
+      </c>
+      <c r="F90">
+        <f>F89/SQRT(6)</f>
+        <v>1.6643446891206011</v>
+      </c>
+      <c r="G90">
+        <f>G89/SQRT(6)</f>
+        <v>1.6643446891206011</v>
+      </c>
+      <c r="H90">
+        <f>H89/SQRT(6)</f>
+        <v>1.6643446891206011</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
+      <c r="B96" t="s">
+        <v>35</v>
+      </c>
+      <c r="C96" t="s">
+        <v>29</v>
+      </c>
+      <c r="D96" t="s">
+        <v>32</v>
+      </c>
+      <c r="E96" t="s">
+        <v>29</v>
+      </c>
+      <c r="F96" t="s">
+        <v>33</v>
+      </c>
+      <c r="G96" t="s">
+        <v>29</v>
+      </c>
+      <c r="H96" t="s">
+        <v>34</v>
+      </c>
+      <c r="I96" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
+      <c r="A97" t="s">
+        <v>1</v>
+      </c>
+      <c r="B97">
+        <v>685</v>
+      </c>
+      <c r="C97">
+        <v>7.11</v>
+      </c>
+      <c r="D97">
+        <v>630</v>
+      </c>
+      <c r="E97">
+        <v>3.23</v>
+      </c>
+      <c r="F97">
+        <v>701.83</v>
+      </c>
+      <c r="G97">
+        <v>16.36</v>
+      </c>
+      <c r="H97">
+        <v>804</v>
+      </c>
+      <c r="I97">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
+      <c r="A98" t="s">
+        <v>2</v>
+      </c>
+      <c r="B98">
+        <v>641</v>
+      </c>
+      <c r="C98">
+        <v>1.66</v>
+      </c>
+      <c r="D98">
+        <v>609</v>
+      </c>
+      <c r="E98">
+        <v>6.14</v>
+      </c>
+      <c r="F98">
+        <v>583.33000000000004</v>
+      </c>
+      <c r="G98">
+        <v>3.38</v>
+      </c>
+      <c r="H98">
+        <v>641</v>
+      </c>
+      <c r="I98">
+        <v>4.24</v>
+      </c>
+    </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
2 bigjobs/2 machine data
git-svn-id: file://localhost/tmp/svn2git/svn@2999 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/async-re/data/Refined_data.xlsx
+++ b/papers/async-re/data/Refined_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
   <si>
     <t>Synchronous</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -137,27 +137,71 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>gap b/w 1st and last bjs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1BJ 8 Reps/32 exchanges</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1BJ 16 Reps/64 ex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4BJs, 4Machines - 16 replicas/64 exchanges</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">2BJS 2 MACHINES </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERIC, LOUIE, OLIVER, POSEIDON, OLIVER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXP#</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gap b/w 1st and lst bjs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>diff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>se</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>decent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2BJs 2Machines, 8 replicas, 32 exchanges</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>SE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>gap b/w 1st and last bjs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1BJ 8 Reps/32 exchanges</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1BJ 16 Reps/64 ex</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1BJ 32 Reps/128 ex</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4BJs, 4Machines - 16 replicas/64 exchanges</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -551,24 +595,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="464178680"/>
-        <c:axId val="478299880"/>
+        <c:axId val="605228296"/>
+        <c:axId val="605718024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="464178680"/>
+        <c:axId val="605228296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="478299880"/>
+        <c:crossAx val="605718024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="478299880"/>
+        <c:axId val="605718024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -576,7 +620,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="464178680"/>
+        <c:crossAx val="605228296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -913,11 +957,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="501251624"/>
-        <c:axId val="478372568"/>
+        <c:axId val="473330520"/>
+        <c:axId val="477341704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="501251624"/>
+        <c:axId val="473330520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -941,14 +985,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="478372568"/>
+        <c:crossAx val="477341704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="478372568"/>
+        <c:axId val="477341704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -956,7 +1000,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="501251624"/>
+        <c:crossAx val="473330520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -981,24 +1025,6 @@
   <c:lang val="en-US"/>
   <c:style val="18"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>LONI machines</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -1031,13 +1057,13 @@
                     <c:v>7.11</c:v>
                   </c:pt>
                   <c:pt idx="1">
+                    <c:v>16.36</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5.57</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
                     <c:v>3.23</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>16.36</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>13.4</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1052,13 +1078,13 @@
                     <c:v>7.11</c:v>
                   </c:pt>
                   <c:pt idx="1">
+                    <c:v>16.36</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5.57</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
                     <c:v>3.23</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>16.36</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>13.4</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1073,13 +1099,13 @@
                   <c:v>4BJs, 4Machines - 16 replicas/64 exchanges</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1BJ 16 Reps/64 ex</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2BJs 2Machines, 8 replicas, 32 exchanges</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1BJ 8 Reps/32 exchanges</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1BJ 16 Reps/64 ex</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1BJ 32 Reps/128 ex</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1094,13 +1120,13 @@
                   <c:v>685.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>701.83</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>632.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>630.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>701.83</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>804.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1133,13 +1159,13 @@
                     <c:v>1.66</c:v>
                   </c:pt>
                   <c:pt idx="1">
+                    <c:v>3.38</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9.17</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
                     <c:v>6.14</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>3.38</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>4.24</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1154,13 +1180,13 @@
                     <c:v>1.66</c:v>
                   </c:pt>
                   <c:pt idx="1">
+                    <c:v>3.38</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9.17</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
                     <c:v>6.14</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>3.38</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>4.24</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1175,13 +1201,13 @@
                   <c:v>4BJs, 4Machines - 16 replicas/64 exchanges</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1BJ 16 Reps/64 ex</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2BJs 2Machines, 8 replicas, 32 exchanges</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1BJ 8 Reps/32 exchanges</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1BJ 16 Reps/64 ex</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1BJ 32 Reps/128 ex</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1196,62 +1222,44 @@
                   <c:v>641.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>583.33</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>607.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>609.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>583.33</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>641.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="524606536"/>
-        <c:axId val="524797800"/>
+        <c:axId val="521845208"/>
+        <c:axId val="479370824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="524606536"/>
+        <c:axId val="521845208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="524797800"/>
+        <c:crossAx val="479370824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="524797800"/>
+        <c:axId val="479370824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Mean runtime, seconds</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="524606536"/>
+        <c:crossAx val="521845208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1334,20 +1342,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>111</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvPr id="6" name="Chart 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2128,10 +2136,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:K98"/>
+  <dimension ref="A1:K123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="M73" sqref="M73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H149" sqref="H149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -2433,7 +2441,7 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B76">
         <v>50</v>
@@ -2776,7 +2784,7 @@
     </row>
     <row r="96" spans="1:9">
       <c r="B96" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C96" t="s">
         <v>29</v>
@@ -2785,19 +2793,19 @@
         <v>32</v>
       </c>
       <c r="E96" t="s">
+        <v>3</v>
+      </c>
+      <c r="F96" t="s">
+        <v>45</v>
+      </c>
+      <c r="G96" t="s">
+        <v>46</v>
+      </c>
+      <c r="H96" t="s">
+        <v>31</v>
+      </c>
+      <c r="I96" t="s">
         <v>29</v>
-      </c>
-      <c r="F96" t="s">
-        <v>33</v>
-      </c>
-      <c r="G96" t="s">
-        <v>29</v>
-      </c>
-      <c r="H96" t="s">
-        <v>34</v>
-      </c>
-      <c r="I96" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -2811,22 +2819,22 @@
         <v>7.11</v>
       </c>
       <c r="D97">
+        <v>701.83</v>
+      </c>
+      <c r="E97">
+        <v>16.36</v>
+      </c>
+      <c r="F97">
+        <v>632</v>
+      </c>
+      <c r="G97">
+        <v>5.57</v>
+      </c>
+      <c r="H97">
         <v>630</v>
       </c>
-      <c r="E97">
+      <c r="I97">
         <v>3.23</v>
-      </c>
-      <c r="F97">
-        <v>701.83</v>
-      </c>
-      <c r="G97">
-        <v>16.36</v>
-      </c>
-      <c r="H97">
-        <v>804</v>
-      </c>
-      <c r="I97">
-        <v>13.4</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -2840,22 +2848,468 @@
         <v>1.66</v>
       </c>
       <c r="D98">
+        <v>583.33000000000004</v>
+      </c>
+      <c r="E98">
+        <v>3.38</v>
+      </c>
+      <c r="F98">
+        <v>607.79999999999995</v>
+      </c>
+      <c r="G98">
+        <v>9.17</v>
+      </c>
+      <c r="H98">
         <v>609</v>
       </c>
-      <c r="E98">
+      <c r="I98">
         <v>6.14</v>
       </c>
-      <c r="F98">
-        <v>583.33000000000004</v>
-      </c>
-      <c r="G98">
-        <v>3.38</v>
-      </c>
-      <c r="H98">
-        <v>641</v>
-      </c>
-      <c r="I98">
-        <v>4.24</v>
+    </row>
+    <row r="106" spans="1:9">
+      <c r="A106" t="s">
+        <v>34</v>
+      </c>
+      <c r="C106" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9">
+      <c r="A108" t="s">
+        <v>36</v>
+      </c>
+      <c r="B108">
+        <v>72</v>
+      </c>
+      <c r="C108">
+        <v>73</v>
+      </c>
+      <c r="D108">
+        <v>74</v>
+      </c>
+      <c r="E108">
+        <v>75</v>
+      </c>
+      <c r="F108">
+        <v>76</v>
+      </c>
+      <c r="G108">
+        <v>77</v>
+      </c>
+      <c r="H108">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9">
+      <c r="A109" t="s">
+        <v>37</v>
+      </c>
+      <c r="B109">
+        <v>17</v>
+      </c>
+      <c r="C109">
+        <v>18</v>
+      </c>
+      <c r="D109">
+        <v>31</v>
+      </c>
+      <c r="E109">
+        <v>12</v>
+      </c>
+      <c r="F109">
+        <v>43</v>
+      </c>
+      <c r="G109">
+        <v>4</v>
+      </c>
+      <c r="H109">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9">
+      <c r="A110" t="s">
+        <v>38</v>
+      </c>
+      <c r="B110">
+        <v>632</v>
+      </c>
+      <c r="C110">
+        <v>637</v>
+      </c>
+      <c r="D110">
+        <v>628</v>
+      </c>
+      <c r="E110">
+        <v>633</v>
+      </c>
+      <c r="F110">
+        <v>645</v>
+      </c>
+      <c r="G110">
+        <v>600</v>
+      </c>
+      <c r="H110">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9">
+      <c r="A111" t="s">
+        <v>39</v>
+      </c>
+      <c r="B111">
+        <v>632</v>
+      </c>
+      <c r="C111">
+        <v>632</v>
+      </c>
+      <c r="D111">
+        <v>632</v>
+      </c>
+      <c r="E111">
+        <v>632</v>
+      </c>
+      <c r="F111">
+        <v>632</v>
+      </c>
+      <c r="G111">
+        <v>632</v>
+      </c>
+      <c r="H111">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9">
+      <c r="A112" t="s">
+        <v>40</v>
+      </c>
+      <c r="B112">
+        <f>(B110-B111)*(B110-B111)</f>
+        <v>0</v>
+      </c>
+      <c r="C112">
+        <f t="shared" ref="C112:H112" si="4">(C110-C111)*(C110-C111)</f>
+        <v>25</v>
+      </c>
+      <c r="D112">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="E112">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F112">
+        <f t="shared" si="4"/>
+        <v>169</v>
+      </c>
+      <c r="G112">
+        <f t="shared" si="4"/>
+        <v>1024</v>
+      </c>
+      <c r="H112">
+        <f t="shared" si="4"/>
+        <v>289</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10">
+      <c r="A113" t="s">
+        <v>41</v>
+      </c>
+      <c r="B113">
+        <v>14.755144381343264</v>
+      </c>
+      <c r="C113">
+        <v>14.755144381343264</v>
+      </c>
+      <c r="D113">
+        <v>14.755144381343264</v>
+      </c>
+      <c r="E113">
+        <v>14.755144381343264</v>
+      </c>
+      <c r="F113">
+        <v>14.755144381343264</v>
+      </c>
+      <c r="G113">
+        <v>14.755144381343264</v>
+      </c>
+      <c r="H113">
+        <v>14.755144381343264</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10">
+      <c r="A114" t="s">
+        <v>42</v>
+      </c>
+      <c r="B114">
+        <f>B113/SQRT(7)</f>
+        <v>5.576920370269467</v>
+      </c>
+      <c r="C114">
+        <f t="shared" ref="C114:H114" si="5">C113/SQRT(7)</f>
+        <v>5.576920370269467</v>
+      </c>
+      <c r="D114">
+        <f t="shared" si="5"/>
+        <v>5.576920370269467</v>
+      </c>
+      <c r="E114">
+        <f t="shared" si="5"/>
+        <v>5.576920370269467</v>
+      </c>
+      <c r="F114">
+        <f t="shared" si="5"/>
+        <v>5.576920370269467</v>
+      </c>
+      <c r="G114">
+        <f t="shared" si="5"/>
+        <v>5.576920370269467</v>
+      </c>
+      <c r="H114">
+        <f t="shared" si="5"/>
+        <v>5.576920370269467</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10">
+      <c r="A117" t="s">
+        <v>36</v>
+      </c>
+      <c r="B117">
+        <v>68</v>
+      </c>
+      <c r="C117">
+        <v>69</v>
+      </c>
+      <c r="D117">
+        <v>70</v>
+      </c>
+      <c r="E117">
+        <v>71</v>
+      </c>
+      <c r="F117">
+        <v>72</v>
+      </c>
+      <c r="G117">
+        <v>73</v>
+      </c>
+      <c r="H117">
+        <v>74</v>
+      </c>
+      <c r="I117">
+        <v>75</v>
+      </c>
+      <c r="J117">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10">
+      <c r="A118" t="s">
+        <v>43</v>
+      </c>
+      <c r="B118">
+        <v>54</v>
+      </c>
+      <c r="C118">
+        <v>33</v>
+      </c>
+      <c r="D118">
+        <v>45</v>
+      </c>
+      <c r="E118">
+        <v>5</v>
+      </c>
+      <c r="F118">
+        <v>13</v>
+      </c>
+      <c r="G118">
+        <v>20</v>
+      </c>
+      <c r="H118">
+        <v>41</v>
+      </c>
+      <c r="I118">
+        <v>38</v>
+      </c>
+      <c r="J118">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10">
+      <c r="A119" t="s">
+        <v>44</v>
+      </c>
+      <c r="B119">
+        <v>621</v>
+      </c>
+      <c r="C119">
+        <v>608</v>
+      </c>
+      <c r="D119">
+        <v>662</v>
+      </c>
+      <c r="E119">
+        <v>586</v>
+      </c>
+      <c r="F119">
+        <v>592</v>
+      </c>
+      <c r="G119">
+        <v>571</v>
+      </c>
+      <c r="H119">
+        <v>622</v>
+      </c>
+      <c r="I119">
+        <v>631</v>
+      </c>
+      <c r="J119">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10">
+      <c r="A120" t="s">
+        <v>25</v>
+      </c>
+      <c r="B120">
+        <v>607.88888888888891</v>
+      </c>
+      <c r="C120">
+        <v>607.88888888888891</v>
+      </c>
+      <c r="D120">
+        <v>607.88888888888891</v>
+      </c>
+      <c r="E120">
+        <v>607.88888888888891</v>
+      </c>
+      <c r="F120">
+        <v>607.88888888888891</v>
+      </c>
+      <c r="G120">
+        <v>607.88888888888891</v>
+      </c>
+      <c r="H120">
+        <v>607.88888888888891</v>
+      </c>
+      <c r="I120">
+        <v>607.88888888888891</v>
+      </c>
+      <c r="J120">
+        <v>607.88888888888891</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10">
+      <c r="A121" t="s">
+        <v>26</v>
+      </c>
+      <c r="B121">
+        <f>(B119-B120)*(B119-B120)</f>
+        <v>171.90123456790056</v>
+      </c>
+      <c r="C121">
+        <f t="shared" ref="C121:J121" si="6">(C119-C120)*(C119-C120)</f>
+        <v>1.2345679012340065E-2</v>
+      </c>
+      <c r="D121">
+        <f t="shared" si="6"/>
+        <v>2928.0123456790097</v>
+      </c>
+      <c r="E121">
+        <f t="shared" si="6"/>
+        <v>479.12345679012458</v>
+      </c>
+      <c r="F121">
+        <f t="shared" si="6"/>
+        <v>252.45679012345758</v>
+      </c>
+      <c r="G121">
+        <f t="shared" si="6"/>
+        <v>1360.7901234567919</v>
+      </c>
+      <c r="H121">
+        <f t="shared" si="6"/>
+        <v>199.12345679012273</v>
+      </c>
+      <c r="I121">
+        <f t="shared" si="6"/>
+        <v>534.1234567901223</v>
+      </c>
+      <c r="J121">
+        <f t="shared" si="6"/>
+        <v>893.3456790123472</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10">
+      <c r="A122" t="s">
+        <v>27</v>
+      </c>
+      <c r="B122">
+        <v>27.525521266411182</v>
+      </c>
+      <c r="C122">
+        <v>27.525521266411182</v>
+      </c>
+      <c r="D122">
+        <v>27.525521266411182</v>
+      </c>
+      <c r="E122">
+        <v>27.525521266411182</v>
+      </c>
+      <c r="F122">
+        <v>27.525521266411182</v>
+      </c>
+      <c r="G122">
+        <v>27.525521266411182</v>
+      </c>
+      <c r="H122">
+        <v>27.525521266411182</v>
+      </c>
+      <c r="I122">
+        <v>27.525521266411182</v>
+      </c>
+      <c r="J122">
+        <v>27.525521266411182</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10">
+      <c r="A123" t="s">
+        <v>28</v>
+      </c>
+      <c r="B123">
+        <f>B122/3</f>
+        <v>9.1751737554703947</v>
+      </c>
+      <c r="C123">
+        <f t="shared" ref="C123:J123" si="7">C122/3</f>
+        <v>9.1751737554703947</v>
+      </c>
+      <c r="D123">
+        <f t="shared" si="7"/>
+        <v>9.1751737554703947</v>
+      </c>
+      <c r="E123">
+        <f t="shared" si="7"/>
+        <v>9.1751737554703947</v>
+      </c>
+      <c r="F123">
+        <f t="shared" si="7"/>
+        <v>9.1751737554703947</v>
+      </c>
+      <c r="G123">
+        <f t="shared" si="7"/>
+        <v>9.1751737554703947</v>
+      </c>
+      <c r="H123">
+        <f t="shared" si="7"/>
+        <v>9.1751737554703947</v>
+      </c>
+      <c r="I123">
+        <f t="shared" si="7"/>
+        <v>9.1751737554703947</v>
+      </c>
+      <c r="J123">
+        <f t="shared" si="7"/>
+        <v>9.1751737554703947</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some more data(64 replica - sync)
git-svn-id: file://localhost/tmp/svn2git/svn@3054 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/async-re/data/Refined_data.xlsx
+++ b/papers/async-re/data/Refined_data.xlsx
@@ -267,6 +267,9 @@
                 <c:pt idx="3">
                   <c:v>1023.0</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>4358.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -520,24 +523,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="495801048"/>
-        <c:axId val="495802376"/>
+        <c:axId val="493451560"/>
+        <c:axId val="451595432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="495801048"/>
+        <c:axId val="493451560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="495802376"/>
+        <c:crossAx val="451595432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="495802376"/>
+        <c:axId val="451595432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -545,7 +548,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="495801048"/>
+        <c:crossAx val="493451560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -785,24 +788,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="493027512"/>
-        <c:axId val="518987256"/>
+        <c:axId val="448863960"/>
+        <c:axId val="465778184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="493027512"/>
+        <c:axId val="448863960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="518987256"/>
+        <c:crossAx val="465778184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="518987256"/>
+        <c:axId val="465778184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -810,7 +813,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="493027512"/>
+        <c:crossAx val="448863960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1217,7 +1220,7 @@
   <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1300,6 +1303,9 @@
       <c r="I3">
         <v>18.34</v>
       </c>
+      <c r="J3">
+        <v>4358</v>
+      </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
@@ -1461,7 +1467,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
cost of dist exchanges
git-svn-id: file://localhost/tmp/svn2git/svn@3058 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/async-re/data/Refined_data.xlsx
+++ b/papers/async-re/data/Refined_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>Synchronous</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -130,6 +130,26 @@
   </si>
   <si>
     <t>#### = no contact</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>w`</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of ex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sync</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>decent</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -559,24 +579,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="471787704"/>
-        <c:axId val="69795112"/>
+        <c:axId val="505651880"/>
+        <c:axId val="505433416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="471787704"/>
+        <c:axId val="505651880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69795112"/>
+        <c:crossAx val="505433416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69795112"/>
+        <c:axId val="505433416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -584,7 +604,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="471787704"/>
+        <c:crossAx val="505651880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -824,24 +844,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="69853368"/>
-        <c:axId val="69840744"/>
+        <c:axId val="505196184"/>
+        <c:axId val="494242616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="69853368"/>
+        <c:axId val="505196184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69840744"/>
+        <c:crossAx val="494242616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69840744"/>
+        <c:axId val="494242616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -849,7 +869,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69853368"/>
+        <c:crossAx val="505196184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1253,10 +1273,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:S97"/>
+  <dimension ref="A1:S105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62:T100"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="K105" sqref="K105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1422,6 +1442,11 @@
         <v>985</v>
       </c>
     </row>
+    <row r="22" spans="14:14">
+      <c r="N22" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>9</v>
@@ -1534,7 +1559,7 @@
         <v>7</v>
       </c>
       <c r="J64" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="K64" t="s">
         <v>22</v>
@@ -2269,15 +2294,172 @@
         <v>26</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:10">
       <c r="A97" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="B101">
+        <v>16</v>
+      </c>
+      <c r="C101">
+        <v>32</v>
+      </c>
+      <c r="D101">
+        <v>64</v>
+      </c>
+      <c r="E101">
+        <v>128</v>
+      </c>
+      <c r="F101">
+        <v>256</v>
+      </c>
+      <c r="G101">
+        <v>512</v>
+      </c>
+      <c r="H101">
+        <v>1024</v>
+      </c>
+      <c r="I101">
+        <v>2048</v>
+      </c>
+      <c r="J101">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="B102">
+        <v>4</v>
+      </c>
+      <c r="C102">
+        <v>8</v>
+      </c>
+      <c r="D102">
+        <v>16</v>
+      </c>
+      <c r="E102">
+        <v>32</v>
+      </c>
+      <c r="F102">
+        <v>64</v>
+      </c>
+      <c r="G102">
+        <v>128</v>
+      </c>
+      <c r="H102">
+        <v>256</v>
+      </c>
+      <c r="I102">
+        <v>512</v>
+      </c>
+      <c r="J102">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10">
+      <c r="A103" t="s">
+        <v>30</v>
+      </c>
+      <c r="B103">
+        <v>32</v>
+      </c>
+      <c r="C103">
+        <v>64</v>
+      </c>
+      <c r="D103">
+        <v>128</v>
+      </c>
+      <c r="E103">
+        <v>256</v>
+      </c>
+      <c r="F103">
+        <v>512</v>
+      </c>
+      <c r="G103">
+        <v>1024</v>
+      </c>
+      <c r="H103">
+        <v>2048</v>
+      </c>
+      <c r="I103">
+        <v>4096</v>
+      </c>
+      <c r="J103">
+        <f>4096*2</f>
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10">
+      <c r="A104" t="s">
+        <v>31</v>
+      </c>
+      <c r="B104">
+        <v>32</v>
+      </c>
+      <c r="C104">
+        <v>64</v>
+      </c>
+      <c r="D104">
+        <v>128</v>
+      </c>
+      <c r="E104">
+        <v>256</v>
+      </c>
+      <c r="F104">
+        <v>512</v>
+      </c>
+      <c r="G104">
+        <v>1024</v>
+      </c>
+      <c r="H104">
+        <v>2048</v>
+      </c>
+      <c r="I104">
+        <v>4096</v>
+      </c>
+      <c r="J104">
+        <f>4096*2</f>
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10">
+      <c r="A105" t="s">
+        <v>32</v>
+      </c>
+      <c r="B105">
+        <v>0</v>
+      </c>
+      <c r="C105">
+        <v>0</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+      <c r="E105">
+        <v>0</v>
+      </c>
+      <c r="F105">
+        <v>0</v>
+      </c>
+      <c r="G105">
+        <v>0</v>
+      </c>
+      <c r="H105">
+        <v>0</v>
+      </c>
+      <c r="I105">
+        <v>0</v>
+      </c>
+      <c r="J105">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
corrections - control flows
git-svn-id: file://localhost/tmp/svn2git/svn@3127 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/async-re/data/Refined_data.xlsx
+++ b/papers/async-re/data/Refined_data.xlsx
@@ -580,24 +580,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="518901784"/>
-        <c:axId val="493096664"/>
+        <c:axId val="491340376"/>
+        <c:axId val="505621736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="518901784"/>
+        <c:axId val="491340376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="493096664"/>
+        <c:crossAx val="505621736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="493096664"/>
+        <c:axId val="505621736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -605,7 +605,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="518901784"/>
+        <c:crossAx val="491340376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -646,7 +646,7 @@
             <c:errValType val="cust"/>
             <c:plus>
               <c:numRef>
-                <c:f>(Sheet1!$C$43,Sheet1!$E$43)</c:f>
+                <c:f>(Sheet1!$B$43,Sheet1!$C$43)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
@@ -661,7 +661,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>(Sheet1!$C$43,Sheet1!$E$43)</c:f>
+                <c:f>(Sheet1!$B$43,Sheet1!$C$43)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
@@ -716,7 +716,7 @@
             <c:errValType val="cust"/>
             <c:plus>
               <c:numRef>
-                <c:f>(Sheet1!$C$44,Sheet1!$E$44)</c:f>
+                <c:f>(Sheet1!$B$44,Sheet1!$C$44)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
@@ -731,7 +731,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>(Sheet1!$C$44,Sheet1!$E$44)</c:f>
+                <c:f>(Sheet1!$B$44,Sheet1!$C$44)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
@@ -786,7 +786,7 @@
             <c:errValType val="cust"/>
             <c:plus>
               <c:numRef>
-                <c:f>(Sheet1!$C$45,Sheet1!$E$45)</c:f>
+                <c:f>(Sheet1!$B$45,Sheet1!$C$45)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
@@ -801,7 +801,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>(Sheet1!$C$45,Sheet1!$E$45)</c:f>
+                <c:f>(Sheet1!$B$45,Sheet1!$C$45)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
@@ -845,24 +845,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="471732264"/>
-        <c:axId val="586471160"/>
+        <c:axId val="451698152"/>
+        <c:axId val="505791784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="471732264"/>
+        <c:axId val="451698152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="586471160"/>
+        <c:crossAx val="505791784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="586471160"/>
+        <c:axId val="505791784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -870,7 +870,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="471732264"/>
+        <c:crossAx val="451698152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -893,16 +893,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1277,7 +1277,7 @@
   <dimension ref="A1:Q105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1446,12 +1446,12 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:3">
       <c r="B38" t="s">
         <v>12</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>1</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>2</v>
       </c>
@@ -1492,35 +1492,35 @@
         <v>607.79999999999995</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:3">
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
       <c r="C42" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:3">
+      <c r="B43">
+        <v>14.5</v>
+      </c>
       <c r="C43">
-        <v>14.5</v>
-      </c>
-      <c r="E43">
         <v>10.050000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:3">
+      <c r="B44">
+        <v>7.11</v>
+      </c>
       <c r="C44">
-        <v>7.11</v>
-      </c>
-      <c r="E44">
         <v>5.57</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:3">
+      <c r="B45">
+        <v>1.66</v>
+      </c>
       <c r="C45">
-        <v>1.66</v>
-      </c>
-      <c r="E45">
         <v>9.17</v>
       </c>
     </row>
@@ -2301,9 +2301,9 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
changes to the excel sheet
git-svn-id: file://localhost/tmp/svn2git/svn@3128 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/async-re/data/Refined_data.xlsx
+++ b/papers/async-re/data/Refined_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
   <si>
     <t>Synchronous</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -580,24 +580,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="491340376"/>
-        <c:axId val="505621736"/>
+        <c:axId val="494558024"/>
+        <c:axId val="505195784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="491340376"/>
+        <c:axId val="494558024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="505621736"/>
+        <c:crossAx val="505195784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="505621736"/>
+        <c:axId val="505195784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -605,7 +605,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="491340376"/>
+        <c:crossAx val="494558024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -845,24 +845,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="451698152"/>
-        <c:axId val="505791784"/>
+        <c:axId val="469486312"/>
+        <c:axId val="518423016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="451698152"/>
+        <c:axId val="469486312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="505791784"/>
+        <c:crossAx val="518423016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="505791784"/>
+        <c:axId val="518423016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -870,7 +870,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="451698152"/>
+        <c:crossAx val="469486312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1276,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:Q105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1524,6 +1524,71 @@
         <v>9.17</v>
       </c>
     </row>
+    <row r="52" spans="1:9">
+      <c r="B52" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52" t="s">
+        <v>3</v>
+      </c>
+      <c r="D52" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53">
+        <v>805</v>
+      </c>
+      <c r="C53">
+        <v>14.5</v>
+      </c>
+      <c r="D53">
+        <v>1179.8</v>
+      </c>
+      <c r="E53">
+        <v>10.050000000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54">
+        <v>632</v>
+      </c>
+      <c r="C54">
+        <v>7.11</v>
+      </c>
+      <c r="D54">
+        <v>685</v>
+      </c>
+      <c r="E54">
+        <v>5.57</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55">
+        <v>607.79999999999995</v>
+      </c>
+      <c r="C55">
+        <v>1.66</v>
+      </c>
+      <c r="D55">
+        <v>641</v>
+      </c>
+      <c r="E55">
+        <v>9.17</v>
+      </c>
+    </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
         <v>19</v>
@@ -2301,6 +2366,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
some changes to the graphs
git-svn-id: file://localhost/tmp/svn2git/svn@3130 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/async-re/data/Refined_data.xlsx
+++ b/papers/async-re/data/Refined_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>Synchronous</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -37,26 +37,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4 replicas/16 exchanges</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8 replicas/32 exchanges</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>16/64</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>32/128</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>64/256</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>distributed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -69,26 +49,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4BJs, 4Machines - 16 replicas/64 exchanges</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2BJs 2Machines, 8 replicas, 32 exchanges</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>SE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>128/512</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>256/1024</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">Synchronous </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -145,7 +109,47 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>est</t>
+    <t>4(16)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8(32)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16(64)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>32(128)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>64(256)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>128(512)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>256(1024)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4(1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8(2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16(4)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -189,9 +193,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -231,10 +236,10 @@
             <c:errValType val="cust"/>
             <c:plus>
               <c:numRef>
-                <c:f>(Sheet1!$C$3,Sheet1!$E$3,Sheet1!$G$3,Sheet1!$I$3)</c:f>
+                <c:f>(Sheet1!$C$3,Sheet1!$E$3,Sheet1!$G$3,Sheet1!$I$3,Sheet1!$K$3,Sheet1!$M$3,Sheet1!$O$3)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="4"/>
+                  <c:ptCount val="7"/>
                   <c:pt idx="0">
                     <c:v>8.81</c:v>
                   </c:pt>
@@ -246,16 +251,25 @@
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>18.34</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>50.0</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>50.0</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>50.0</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>(Sheet1!$C$3,Sheet1!$E$3,Sheet1!$G$3,Sheet1!$I$3)</c:f>
+                <c:f>(Sheet1!$C$3,Sheet1!$E$3,Sheet1!$G$3,Sheet1!$I$3,Sheet1!$K$3,Sheet1!$M$3,Sheet1!$O$3)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="4"/>
+                  <c:ptCount val="7"/>
                   <c:pt idx="0">
                     <c:v>8.81</c:v>
                   </c:pt>
@@ -267,6 +281,15 @@
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>18.34</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>50.0</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>50.0</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>50.0</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -278,25 +301,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4 replicas/16 exchanges</c:v>
+                  <c:v>4(16)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8 replicas/32 exchanges</c:v>
+                  <c:v>8(32)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16/64</c:v>
+                  <c:v>16(64)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32/128</c:v>
+                  <c:v>32(128)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>64/256</c:v>
+                  <c:v>64(256)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>128/512</c:v>
+                  <c:v>128(512)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>256/1024</c:v>
+                  <c:v>256(1024)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -351,10 +374,10 @@
             <c:errValType val="cust"/>
             <c:plus>
               <c:numRef>
-                <c:f>(Sheet1!$C$4,Sheet1!$E$4,Sheet1!$G$4,Sheet1!$I$4,Sheet1!$K$4)</c:f>
+                <c:f>(Sheet1!$C$4,Sheet1!$E$4,Sheet1!$G$4,Sheet1!$I$4,Sheet1!$K$4,Sheet1!$M$4,Sheet1!$O$4)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
+                  <c:ptCount val="7"/>
                   <c:pt idx="0">
                     <c:v>11.1</c:v>
                   </c:pt>
@@ -369,16 +392,22 @@
                   </c:pt>
                   <c:pt idx="4">
                     <c:v>19.2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>7.0</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>50.0</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>(Sheet1!$C$4,Sheet1!$E$4,Sheet1!$G$4,Sheet1!$I$4,Sheet1!$K$4)</c:f>
+                <c:f>(Sheet1!$C$4,Sheet1!$E$4,Sheet1!$G$4,Sheet1!$I$4,Sheet1!$K$4,Sheet1!$M$4,Sheet1!$O$4)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
+                  <c:ptCount val="7"/>
                   <c:pt idx="0">
                     <c:v>11.1</c:v>
                   </c:pt>
@@ -393,6 +422,12 @@
                   </c:pt>
                   <c:pt idx="4">
                     <c:v>19.2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>7.0</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>50.0</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -404,25 +439,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4 replicas/16 exchanges</c:v>
+                  <c:v>4(16)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8 replicas/32 exchanges</c:v>
+                  <c:v>8(32)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16/64</c:v>
+                  <c:v>16(64)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32/128</c:v>
+                  <c:v>32(128)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>64/256</c:v>
+                  <c:v>64(256)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>128/512</c:v>
+                  <c:v>128(512)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>256/1024</c:v>
+                  <c:v>256(1024)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -542,25 +577,25 @@
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4 replicas/16 exchanges</c:v>
+                  <c:v>4(16)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8 replicas/32 exchanges</c:v>
+                  <c:v>8(32)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16/64</c:v>
+                  <c:v>16(64)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32/128</c:v>
+                  <c:v>32(128)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>64/256</c:v>
+                  <c:v>64(256)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>128/512</c:v>
+                  <c:v>128(512)</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>256/1024</c:v>
+                  <c:v>256(1024)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -596,32 +631,68 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="491451352"/>
-        <c:axId val="465618136"/>
+        <c:axId val="464952344"/>
+        <c:axId val="488486872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="491451352"/>
+        <c:axId val="464952344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Replicas(Number of Exchanges)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="465618136"/>
+        <c:crossAx val="488486872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="465618136"/>
+        <c:axId val="488486872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Runtime (in seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="491451352"/>
+        <c:crossAx val="464952344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -655,21 +726,32 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Synchronous</c:v>
+            <c:strRef>
+              <c:f>Sheet1!$A$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Synchronous </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
             <c:plus>
               <c:numRef>
-                <c:f>(Sheet1!$B$43,Sheet1!$C$43)</c:f>
+                <c:f>(Sheet1!$C$39,Sheet1!$E$39,Sheet1!$G$39)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="2"/>
+                  <c:ptCount val="3"/>
                   <c:pt idx="0">
+                    <c:v>8.81</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
                     <c:v>14.5</c:v>
                   </c:pt>
-                  <c:pt idx="1">
+                  <c:pt idx="2">
                     <c:v>10.05</c:v>
                   </c:pt>
                 </c:numCache>
@@ -677,14 +759,17 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>(Sheet1!$B$43,Sheet1!$C$43)</c:f>
+                <c:f>(Sheet1!$C$39,Sheet1!$E$39,Sheet1!$G$39)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="2"/>
+                  <c:ptCount val="3"/>
                   <c:pt idx="0">
+                    <c:v>8.81</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
                     <c:v>14.5</c:v>
                   </c:pt>
-                  <c:pt idx="1">
+                  <c:pt idx="2">
                     <c:v>10.05</c:v>
                   </c:pt>
                 </c:numCache>
@@ -693,29 +778,35 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$38:$C$38</c:f>
+              <c:f>(Sheet1!$B$38,Sheet1!$D$38,Sheet1!$F$38)</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4BJs, 4Machines - 16 replicas/64 exchanges</c:v>
+                  <c:v>4(1)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2BJs 2Machines, 8 replicas, 32 exchanges</c:v>
+                  <c:v>8(2)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16(4)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$39:$C$39</c:f>
+              <c:f>(Sheet1!$B$39,Sheet1!$D$39,Sheet1!$F$39)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1179.8</c:v>
+                  <c:v>624.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>805.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1179.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -725,21 +816,32 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Asynchronous-Centralized</c:v>
+            <c:strRef>
+              <c:f>Sheet1!$A$40</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Asynchronous - Centralized</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
             <c:plus>
               <c:numRef>
-                <c:f>(Sheet1!$B$44,Sheet1!$C$44)</c:f>
+                <c:f>(Sheet1!$C$40,Sheet1!$E$40,Sheet1!$G$40)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="2"/>
+                  <c:ptCount val="3"/>
                   <c:pt idx="0">
+                    <c:v>11.1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
                     <c:v>7.11</c:v>
                   </c:pt>
-                  <c:pt idx="1">
+                  <c:pt idx="2">
                     <c:v>5.57</c:v>
                   </c:pt>
                 </c:numCache>
@@ -747,14 +849,17 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>(Sheet1!$B$44,Sheet1!$C$44)</c:f>
+                <c:f>(Sheet1!$C$40,Sheet1!$E$40,Sheet1!$G$40)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="2"/>
+                  <c:ptCount val="3"/>
                   <c:pt idx="0">
+                    <c:v>11.1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
                     <c:v>7.11</c:v>
                   </c:pt>
-                  <c:pt idx="1">
+                  <c:pt idx="2">
                     <c:v>5.57</c:v>
                   </c:pt>
                 </c:numCache>
@@ -763,29 +868,35 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$38:$C$38</c:f>
+              <c:f>(Sheet1!$B$38,Sheet1!$D$38,Sheet1!$F$38)</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4BJs, 4Machines - 16 replicas/64 exchanges</c:v>
+                  <c:v>4(1)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2BJs 2Machines, 8 replicas, 32 exchanges</c:v>
+                  <c:v>8(2)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16(4)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$40:$C$40</c:f>
+              <c:f>(Sheet1!$B$40,Sheet1!$D$40,Sheet1!$F$40)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>685.0</c:v>
+                  <c:v>628.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>632.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>685.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -795,21 +906,32 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Asynchronous-Decentralized</c:v>
+            <c:strRef>
+              <c:f>Sheet1!$A$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Asynchronous - Decentralized</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
             <c:plus>
               <c:numRef>
-                <c:f>(Sheet1!$B$45,Sheet1!$C$45)</c:f>
+                <c:f>(Sheet1!$C$41,Sheet1!$E$41,Sheet1!$G$41)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="2"/>
+                  <c:ptCount val="3"/>
                   <c:pt idx="0">
+                    <c:v>5.97</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
                     <c:v>1.66</c:v>
                   </c:pt>
-                  <c:pt idx="1">
+                  <c:pt idx="2">
                     <c:v>9.17</c:v>
                   </c:pt>
                 </c:numCache>
@@ -817,14 +939,17 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>(Sheet1!$B$45,Sheet1!$C$45)</c:f>
+                <c:f>(Sheet1!$C$41,Sheet1!$E$41,Sheet1!$G$41)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="2"/>
+                  <c:ptCount val="3"/>
                   <c:pt idx="0">
+                    <c:v>5.97</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
                     <c:v>1.66</c:v>
                   </c:pt>
-                  <c:pt idx="1">
+                  <c:pt idx="2">
                     <c:v>9.17</c:v>
                   </c:pt>
                 </c:numCache>
@@ -833,60 +958,102 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$38:$C$38</c:f>
+              <c:f>(Sheet1!$B$38,Sheet1!$D$38,Sheet1!$F$38)</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4BJs, 4Machines - 16 replicas/64 exchanges</c:v>
+                  <c:v>4(1)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2BJs 2Machines, 8 replicas, 32 exchanges</c:v>
+                  <c:v>8(2)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16(4)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$41:$C$41</c:f>
+              <c:f>(Sheet1!$B$41,Sheet1!$D$41,Sheet1!$F$41)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>641.0</c:v>
+                  <c:v>588.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>607.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>641.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="494004424"/>
-        <c:axId val="495111304"/>
+        <c:axId val="518479288"/>
+        <c:axId val="503911160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="494004424"/>
+        <c:axId val="518479288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Replicas(Number of Machines)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="495111304"/>
+        <c:crossAx val="503911160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="495111304"/>
+        <c:axId val="503911160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Runtime (in seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="494004424"/>
+        <c:crossAx val="518479288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -939,20 +1106,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="35" name="Chart 34"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1293,58 +1460,58 @@
   <dimension ref="A1:Q105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="B2" t="s">
-        <v>4</v>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
       </c>
       <c r="H2" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="I2" t="s">
         <v>3</v>
       </c>
       <c r="J2" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="K2" t="s">
         <v>3</v>
       </c>
       <c r="L2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="M2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="N2" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="O2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -1379,20 +1546,20 @@
       <c r="J3">
         <v>1350</v>
       </c>
-      <c r="K3" t="s">
-        <v>31</v>
+      <c r="K3">
+        <v>50</v>
       </c>
       <c r="L3">
         <v>2100</v>
       </c>
-      <c r="M3" t="s">
-        <v>31</v>
+      <c r="M3">
+        <v>50</v>
       </c>
       <c r="N3">
         <v>3200</v>
       </c>
-      <c r="O3" t="s">
-        <v>31</v>
+      <c r="O3">
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -1442,8 +1609,8 @@
       <c r="N4">
         <v>1800</v>
       </c>
-      <c r="O4" t="s">
-        <v>31</v>
+      <c r="O4">
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -1493,160 +1660,111 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="B38" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="C38" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>29</v>
+      </c>
+      <c r="D38" t="s">
+        <v>31</v>
+      </c>
+      <c r="E38" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38" t="s">
+        <v>32</v>
+      </c>
+      <c r="G38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B39">
+        <v>624</v>
+      </c>
+      <c r="C39">
+        <v>8.81</v>
+      </c>
+      <c r="D39">
+        <v>805</v>
+      </c>
+      <c r="E39">
+        <v>14.5</v>
+      </c>
+      <c r="F39">
         <v>1179.8</v>
       </c>
-      <c r="C39">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+      <c r="G39">
+        <v>10.050000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>1</v>
       </c>
       <c r="B40">
+        <v>628.6</v>
+      </c>
+      <c r="C40">
+        <v>11.1</v>
+      </c>
+      <c r="D40">
+        <v>632</v>
+      </c>
+      <c r="E40">
+        <v>7.11</v>
+      </c>
+      <c r="F40">
         <v>685</v>
       </c>
-      <c r="C40">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="G40">
+        <v>5.57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>2</v>
       </c>
       <c r="B41">
+        <v>588.9</v>
+      </c>
+      <c r="C41">
+        <v>5.97</v>
+      </c>
+      <c r="D41">
+        <v>607.79999999999995</v>
+      </c>
+      <c r="E41">
+        <v>1.66</v>
+      </c>
+      <c r="F41">
         <v>641</v>
       </c>
-      <c r="C41">
-        <v>607.79999999999995</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="B42" t="s">
-        <v>11</v>
-      </c>
-      <c r="C42" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="B43">
-        <v>14.5</v>
-      </c>
-      <c r="C43">
-        <v>10.050000000000001</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="B44">
-        <v>7.11</v>
-      </c>
-      <c r="C44">
-        <v>5.57</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="B45">
-        <v>1.66</v>
-      </c>
-      <c r="C45">
-        <v>9.17</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
-      <c r="B52" t="s">
-        <v>13</v>
-      </c>
-      <c r="C52" t="s">
-        <v>3</v>
-      </c>
-      <c r="D52" t="s">
-        <v>12</v>
-      </c>
-      <c r="E52" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
-      <c r="A53" t="s">
-        <v>17</v>
-      </c>
-      <c r="B53">
-        <v>805</v>
-      </c>
-      <c r="C53">
-        <v>14.5</v>
-      </c>
-      <c r="D53">
-        <v>1179.8</v>
-      </c>
-      <c r="E53">
-        <v>10.050000000000001</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
-      <c r="A54" t="s">
-        <v>1</v>
-      </c>
-      <c r="B54">
-        <v>632</v>
-      </c>
-      <c r="C54">
-        <v>7.11</v>
-      </c>
-      <c r="D54">
-        <v>685</v>
-      </c>
-      <c r="E54">
-        <v>5.57</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
-      <c r="A55" t="s">
-        <v>2</v>
-      </c>
-      <c r="B55">
-        <v>607.79999999999995</v>
-      </c>
-      <c r="C55">
-        <v>1.66</v>
-      </c>
-      <c r="D55">
-        <v>641</v>
-      </c>
-      <c r="E55">
+      <c r="G41">
         <v>9.17</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C62" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -1799,15 +1917,15 @@
     </row>
     <row r="76" spans="1:17">
       <c r="A76" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C76" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="78" spans="1:17">
       <c r="A78" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -2066,13 +2184,13 @@
         <v>26</v>
       </c>
       <c r="N83" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="O83">
         <v>67</v>
       </c>
       <c r="P83" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="Q83">
         <v>784</v>
@@ -2211,13 +2329,13 @@
         <v>288</v>
       </c>
       <c r="N88" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="O88" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="P88" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="Q88">
         <v>88</v>
@@ -2231,13 +2349,13 @@
         <v>28</v>
       </c>
       <c r="N89" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="O89" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="P89" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="Q89">
         <v>563</v>
@@ -2257,7 +2375,7 @@
         <v>1009</v>
       </c>
       <c r="Q90" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:17">
@@ -2300,17 +2418,17 @@
     </row>
     <row r="96" spans="1:17">
       <c r="A96" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="97" spans="1:8">
       <c r="A97" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="102" spans="1:8">
       <c r="A102" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B102">
         <v>16</v>
@@ -2336,7 +2454,7 @@
     </row>
     <row r="103" spans="1:8">
       <c r="A103" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B103">
         <v>32</v>
@@ -2362,7 +2480,7 @@
     </row>
     <row r="104" spans="1:8">
       <c r="A104" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B104">
         <v>32</v>
@@ -2388,7 +2506,7 @@
     </row>
     <row r="105" spans="1:8">
       <c r="A105" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B105">
         <v>0</v>
@@ -2415,6 +2533,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
corrections to the data, new graphs in Refined_data_AL and abstract
git-svn-id: file://localhost/tmp/svn2git/svn@3173 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/async-re/data/Refined_data.xlsx
+++ b/papers/async-re/data/Refined_data.xlsx
@@ -274,7 +274,7 @@
                     <c:v>17.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>18.34</c:v>
+                    <c:v>34.0</c:v>
                   </c:pt>
                   <c:pt idx="4">
                     <c:v>50.0</c:v>
@@ -304,7 +304,7 @@
                     <c:v>17.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>18.34</c:v>
+                    <c:v>34.0</c:v>
                   </c:pt>
                   <c:pt idx="4">
                     <c:v>50.0</c:v>
@@ -655,11 +655,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="702359448"/>
-        <c:axId val="702344856"/>
+        <c:axId val="712317384"/>
+        <c:axId val="711586456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="702359448"/>
+        <c:axId val="712317384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -683,14 +683,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="702344856"/>
+        <c:crossAx val="711586456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="702344856"/>
+        <c:axId val="711586456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -716,7 +716,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="702359448"/>
+        <c:crossAx val="712317384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -785,7 +785,7 @@
                     <c:v>3.8</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>18.34</c:v>
+                    <c:v>34.0</c:v>
                   </c:pt>
                   <c:pt idx="6">
                     <c:v>10.0</c:v>
@@ -818,7 +818,7 @@
                     <c:v>3.8</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>18.34</c:v>
+                    <c:v>34.0</c:v>
                   </c:pt>
                   <c:pt idx="6">
                     <c:v>10.0</c:v>
@@ -887,7 +887,7 @@
                   <c:v>1023.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1081.0</c:v>
+                  <c:v>965.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>879.0</c:v>
@@ -1196,11 +1196,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="702807768"/>
-        <c:axId val="703074216"/>
+        <c:axId val="712260776"/>
+        <c:axId val="712251304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="702807768"/>
+        <c:axId val="712260776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1224,14 +1224,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="703074216"/>
+        <c:crossAx val="712251304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="703074216"/>
+        <c:axId val="712251304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1257,7 +1257,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="702807768"/>
+        <c:crossAx val="712260776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1663,8 +1663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:Q105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="N63" sqref="N63"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1745,7 +1745,7 @@
         <v>1023</v>
       </c>
       <c r="I3">
-        <v>18.34</v>
+        <v>34</v>
       </c>
       <c r="J3">
         <v>1350</v>
@@ -1958,10 +1958,10 @@
         <v>1023</v>
       </c>
       <c r="M39">
-        <v>18.34</v>
+        <v>34</v>
       </c>
       <c r="N39">
-        <v>1081</v>
+        <v>965</v>
       </c>
       <c r="O39">
         <v>10</v>
@@ -2857,10 +2857,8 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>